<commit_message>
Se realizo scraping a cada de las url del excel y se almaceno de cada uno en un archivo txt
</commit_message>
<xml_diff>
--- a/Web-Scrapi/excelResultProfundo/0.0.urls_extraidas.xlsx
+++ b/Web-Scrapi/excelResultProfundo/0.0.urls_extraidas.xlsx
@@ -19,235 +19,235 @@
     <t>URL</t>
   </si>
   <si>
+    <t>https://da.wikipedia.org/wiki/End-to-end-kryptering</t>
+  </si>
+  <si>
+    <t>https://arstechnica.com/security/2013/05/think-your-skype-messages-get-end-to-end-encryption-think-again/</t>
+  </si>
+  <si>
+    <t>https://zu.wikipedia.org/wiki/Unyandla_olungungiwe</t>
+  </si>
+  <si>
+    <t>https://www.eff.org/deeplinks/2016/04/whatsapp-rolls-out-end-end-encryption-its-1bn-users</t>
+  </si>
+  <si>
+    <t>http://www.businessinsider.com/googles-project-vault-for-secret-messages-2015-5?r=US&amp;amp;IR=T&amp;amp;IR=T</t>
+  </si>
+  <si>
+    <t>https://tr.wikipedia.org/wiki/U%C3%A7tan_uca_%C5%9Fifreleme</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20160120015142/https://ssd.eff.org/en/module/how-use-otr-windows</t>
+  </si>
+  <si>
+    <t>https://eu.wikipedia.org/wiki/Ertzetik_ertzerako_zifratze</t>
+  </si>
+  <si>
+    <t>https://pep.foundation/docs/pEp-whitepaper.pdf</t>
+  </si>
+  <si>
+    <t>https://pl.wikipedia.org/wiki/Szyfrowanie_od_ko%C5%84ca_do_ko%C5%84ca</t>
+  </si>
+  <si>
+    <t>https://foundation.wikimedia.org/wiki/Special:MyLanguage/Policy:Cookie_statement/es</t>
+  </si>
+  <si>
+    <t>https://www.whonix.org/wiki/Air_Gapped_OpenPGP_Key</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/1999/xlink</t>
+  </si>
+  <si>
+    <t>https://cypherpunks.ca/~iang/pubs/impauth.pdf</t>
+  </si>
+  <si>
+    <t>https://www.schneier.com/blog/archives/2013/10/air_gaps.html</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Crittografia_end-to-end</t>
+  </si>
+  <si>
+    <t>https://uk.wikipedia.org/wiki/%D0%9D%D0%B0%D1%81%D0%BA%D1%80%D1%96%D0%B7%D0%BD%D0%B5_%D1%88%D0%B8%D1%84%D1%80%D1%83%D0%B2%D0%B0%D0%BD%D0%BD%D1%8F</t>
+  </si>
+  <si>
+    <t>https://www.wired.com/2014/11/hacker-lexicon-end-to-end-encryption/</t>
+  </si>
+  <si>
+    <t>https://pt.wikipedia.org/wiki/Criptografia_de_ponta-a-ponta</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%A1%D0%BA%D0%B2%D0%BE%D0%B7%D0%BD%D0%BE%D0%B5_%D1%88%D0%B8%D1%84%D1%80%D0%BE%D0%B2%D0%B0%D0%BD%D0%B8%D0%B5</t>
+  </si>
+  <si>
+    <t>https://cpj.org/blog/2016/05/why-telegrams-security-flaws-may-put-irans-journal.php</t>
+  </si>
+  <si>
+    <t>https://ja.wikipedia.org/wiki/%E3%82%A8%E3%83%B3%E3%83%89%E3%83%84%E3%83%BC%E3%82%A8%E3%83%B3%E3%83%89%E6%9A%97%E5%8F%B7%E5%8C%96</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20161001160110/https://pep.foundation/docs/pEp-whitepaper.pdf</t>
+  </si>
+  <si>
+    <t>https://github.com/maqp/tfc</t>
+  </si>
+  <si>
+    <t>https://vi.wikipedia.org/wiki/M%C3%A3_h%C3%B3a_%C4%91%E1%BA%A7u_cu%E1%BB%91i</t>
+  </si>
+  <si>
+    <t>https://www.theguardian.com/world/2013/jul/11/microsoft-nsa-collaboration-user-data</t>
+  </si>
+  <si>
+    <t>https://es.wikipedia.org/w/index.php?title=Cifrado_de_extremo_a_extremo&amp;amp;oldid=163332720&lt;/a</t>
+  </si>
+  <si>
+    <t>https://he.wikipedia.org/wiki/%D7%94%D7%A6%D7%A4%D7%A0%D7%94_%D7%9E%D7%A7%D7%A6%D7%94-%D7%9C%D7%A7%D7%A6%D7%94</t>
+  </si>
+  <si>
+    <t>https://cs.wikipedia.org/wiki/Koncov%C3%A9_%C5%A1ifrov%C3%A1n%C3%AD</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/1999/xlink\</t>
+  </si>
+  <si>
+    <t>https://stats.wikimedia.org/#/es.wikipedia.org</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/1999/xlink%22</t>
+  </si>
+  <si>
+    <t>https://www.mediawiki.org/</t>
+  </si>
+  <si>
+    <t>https://archive.org/details/cryptographyengi00ferg</t>
+  </si>
+  <si>
+    <t>https://blog.cryptographyengineering.com/2013/03/09/here-come-encryption-apps/</t>
+  </si>
+  <si>
+    <t>https://es.wikipedia.org/wiki/Wikipedia:Mes_de_Asia/2024</t>
+  </si>
+  <si>
+    <t>https://www.wired.com/2015/10/mr-robot-uses-protonmail-still-isnt-fully-secure/</t>
+  </si>
+  <si>
+    <t>https://wikimediafoundation.org/</t>
+  </si>
+  <si>
+    <t>http://fortune.com/2016/05/21/google-allo-privacy-2/</t>
+  </si>
+  <si>
+    <t>https://ml.wikipedia.org/wiki/%E0%B4%8E%E0%B5%BB%E0%B4%A1%E0%B5%8D-%E0%B4%9F%E0%B5%81-%E0%B4%8E%E0%B5%BB%E0%B4%A1%E0%B5%8D_%E0%B4%8E%E0%B5%BB%E0%B4%95%E0%B5%8D%E0%B4%B0%E0%B4%BF%E0%B4%AA%E0%B5%8D%E0%B4%B7%E0%B5%BB</t>
+  </si>
+  <si>
+    <t>https://ar.wikipedia.org/wiki/%D8%AA%D8%B9%D9%85%D9%8A%D8%A9_%D8%A8%D9%8A%D9%86_%D8%A7%D9%84%D8%B7%D8%B1%D9%81%D9%8A%D8%A7%D8%AA</t>
+  </si>
+  <si>
     <t>https://sv.wikipedia.org/wiki/Totalstr%C3%A4ckskryptering</t>
   </si>
   <si>
+    <t>https://www.wikidata.org/wiki/Special:EntityPage/Q1340257#sitelinks-wikipedia</t>
+  </si>
+  <si>
+    <t>https://az.wikipedia.org/wiki/Ucdan_uca_%C5%9Fifr%C9%99l%C9%99m%C9%99</t>
+  </si>
+  <si>
+    <t>https://id.wikipedia.org/wiki/Enkripsi_ujung_ke_ujung</t>
+  </si>
+  <si>
+    <t>https://developer.wikimedia.org</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/8/86/Wikipedia_Mes_de_Asia_Banner.svg</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q1340257</t>
+  </si>
+  <si>
+    <t>https://ko.wikipedia.org/wiki/%EB%8B%A8%EB%8C%80%EB%8B%A8_%EC%95%94%ED%98%B8%ED%99%94</t>
+  </si>
+  <si>
+    <t>https://zh.wikipedia.org/wiki/%E7%AB%AF%E5%88%B0%E7%AB%AF%E5%8A%A0%E5%AF%86</t>
+  </si>
+  <si>
+    <t>https://foundation.wikimedia.org/wiki/Policy:Privacy_policy/es</t>
+  </si>
+  <si>
     <t>http://www.w3.org/2000/svg\</t>
   </si>
   <si>
-    <t>https://arstechnica.com/security/2013/05/think-your-skype-messages-get-end-to-end-encryption-think-again/</t>
-  </si>
-  <si>
-    <t>https://blog.cryptographyengineering.com/2013/03/09/here-come-encryption-apps/</t>
-  </si>
-  <si>
-    <t>https://uk.wikipedia.org/wiki/%D0%9D%D0%B0%D1%81%D0%BA%D1%80%D1%96%D0%B7%D0%BD%D0%B5_%D1%88%D0%B8%D1%84%D1%80%D1%83%D0%B2%D0%B0%D0%BD%D0%BD%D1%8F</t>
-  </si>
-  <si>
-    <t>https://stats.wikimedia.org/#/es.wikipedia.org</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/1999/xlink%22</t>
+    <t>https://de.wikipedia.org/wiki/Ende-zu-Ende-Verschl%C3%BCsselung</t>
+  </si>
+  <si>
+    <t>http://internetofthingsagenda.techtarget.com/definition/man-in-the-middle-attack-MitM</t>
+  </si>
+  <si>
+    <t>https://zh-yue.wikipedia.org/wiki/%E7%AB%AF%E5%88%B0%E7%AB%AF%E5%8A%A0%E5%AF%86</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/End-to-end_encryption</t>
+  </si>
+  <si>
+    <t>https://es.wikipedia.org/wiki/Cifrado_de_extremo_a_extremo</t>
+  </si>
+  <si>
+    <t>https://foundation.wikimedia.org/wiki/Special:MyLanguage/Policy:Universal_Code_of_Conduct</t>
+  </si>
+  <si>
+    <t>https://whispersystems.org/blog/whatsapp-complete/</t>
+  </si>
+  <si>
+    <t>https://foundation.wikimedia.org/wiki/Special:MyLanguage/Policy:Privacy_policy/es</t>
+  </si>
+  <si>
+    <t>https://fr.wikipedia.org/wiki/Chiffrement_de_bout_en_bout</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by-sa/4.0/deed.es</t>
+  </si>
+  <si>
+    <t>https://foundation.wikimedia.org/wiki/Policy:Terms_of_Use/es</t>
+  </si>
+  <si>
+    <t>https://nl.wikipedia.org/wiki/End-to-end-encryptie</t>
+  </si>
+  <si>
+    <t>https://archive.org/details/cryptographyengi00ferg/page/n211</t>
+  </si>
+  <si>
+    <t>https://dx.doi.org/10.1145%2F1314333.1314340</t>
+  </si>
+  <si>
+    <t>https://login.wikimedia.org/wiki/Special:CentralAutoLogin/start?type=1x1</t>
+  </si>
+  <si>
+    <t>https://ssd.eff.org/en/glossary/end-end-encryption</t>
+  </si>
+  <si>
+    <t>https://es.wikipedia.org/w/index.php?title=Cifrado_de_extremo_a_extremo&amp;amp;oldid=163332720</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2000/svg</t>
+  </si>
+  <si>
+    <t>https://theintercept.com/2015/12/21/democratic-debate-spawns-fantasy-talk-on-encryption/</t>
+  </si>
+  <si>
+    <t>https://ssd.eff.org/en/module/how-use-otr-windows</t>
+  </si>
+  <si>
+    <t>https://fa.wikipedia.org/wiki/%D8%B1%D9%85%D8%B2%DA%AF%D8%B0%D8%A7%D8%B1%DB%8C_%D8%B3%D8%B1%D8%AA%D8%A7%D8%B3%D8%B1</t>
+  </si>
+  <si>
+    <t>https://github.com/maqp/tfc&lt;/a</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2000/svg%22</t>
   </si>
   <si>
     <t>https://wikimediafoundation.org/es/</t>
   </si>
   <si>
-    <t>http://internetofthingsagenda.techtarget.com/definition/man-in-the-middle-attack-MitM</t>
-  </si>
-  <si>
-    <t>https://web.archive.org/web/20160120015142/https://ssd.eff.org/en/module/how-use-otr-windows</t>
-  </si>
-  <si>
-    <t>https://es.wikipedia.org/w/index.php?title=Cifrado_de_extremo_a_extremo&amp;amp;oldid=163332720&lt;/a</t>
-  </si>
-  <si>
-    <t>https://github.com/maqp/tfc</t>
-  </si>
-  <si>
-    <t>https://fr.wikipedia.org/wiki/Chiffrement_de_bout_en_bout</t>
-  </si>
-  <si>
-    <t>https://zu.wikipedia.org/wiki/Unyandla_olungungiwe</t>
-  </si>
-  <si>
-    <t>https://www.wikidata.org/wiki/Q1340257</t>
-  </si>
-  <si>
-    <t>https://ru.wikipedia.org/wiki/%D0%A1%D0%BA%D0%B2%D0%BE%D0%B7%D0%BD%D0%BE%D0%B5_%D1%88%D0%B8%D1%84%D1%80%D0%BE%D0%B2%D0%B0%D0%BD%D0%B8%D0%B5</t>
-  </si>
-  <si>
-    <t>https://whispersystems.org/blog/whatsapp-complete/</t>
-  </si>
-  <si>
-    <t>https://www.eff.org/deeplinks/2016/04/whatsapp-rolls-out-end-end-encryption-its-1bn-users</t>
-  </si>
-  <si>
-    <t>http://www.businessinsider.com/googles-project-vault-for-secret-messages-2015-5?r=US&amp;amp;IR=T&amp;amp;IR=T</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2000/svg%22</t>
-  </si>
-  <si>
-    <t>https://zh-yue.wikipedia.org/wiki/%E7%AB%AF%E5%88%B0%E7%AB%AF%E5%8A%A0%E5%AF%86</t>
-  </si>
-  <si>
-    <t>https://zh.wikipedia.org/wiki/%E7%AB%AF%E5%88%B0%E7%AB%AF%E5%8A%A0%E5%AF%86</t>
-  </si>
-  <si>
-    <t>https://pep.foundation/docs/pEp-whitepaper.pdf</t>
-  </si>
-  <si>
     <t>https://www.wikidata.org/wiki/Special:EntityPage/Q1340257</t>
-  </si>
-  <si>
-    <t>https://ar.wikipedia.org/wiki/%D8%AA%D8%B9%D9%85%D9%8A%D8%A9_%D8%A8%D9%8A%D9%86_%D8%A7%D9%84%D8%B7%D8%B1%D9%81%D9%8A%D8%A7%D8%AA</t>
-  </si>
-  <si>
-    <t>https://fa.wikipedia.org/wiki/%D8%B1%D9%85%D8%B2%DA%AF%D8%B0%D8%A7%D8%B1%DB%8C_%D8%B3%D8%B1%D8%AA%D8%A7%D8%B3%D8%B1</t>
-  </si>
-  <si>
-    <t>https://foundation.wikimedia.org/wiki/Policy:Privacy_policy/es</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/1999/xlink\</t>
-  </si>
-  <si>
-    <t>https://az.wikipedia.org/wiki/Ucdan_uca_%C5%9Fifr%C9%99l%C9%99m%C9%99</t>
-  </si>
-  <si>
-    <t>https://ja.wikipedia.org/wiki/%E3%82%A8%E3%83%B3%E3%83%89%E3%83%84%E3%83%BC%E3%82%A8%E3%83%B3%E3%83%89%E6%9A%97%E5%8F%B7%E5%8C%96</t>
-  </si>
-  <si>
-    <t>https://archive.org/details/cryptographyengi00ferg</t>
-  </si>
-  <si>
-    <t>https://www.wired.com/2014/11/hacker-lexicon-end-to-end-encryption/</t>
-  </si>
-  <si>
-    <t>https://wikimediafoundation.org/</t>
-  </si>
-  <si>
-    <t>https://www.mediawiki.org/</t>
-  </si>
-  <si>
-    <t>https://vi.wikipedia.org/wiki/M%C3%A3_h%C3%B3a_%C4%91%E1%BA%A7u_cu%E1%BB%91i</t>
-  </si>
-  <si>
-    <t>https://ml.wikipedia.org/wiki/%E0%B4%8E%E0%B5%BB%E0%B4%A1%E0%B5%8D-%E0%B4%9F%E0%B5%81-%E0%B4%8E%E0%B5%BB%E0%B4%A1%E0%B5%8D_%E0%B4%8E%E0%B5%BB%E0%B4%95%E0%B5%8D%E0%B4%B0%E0%B4%BF%E0%B4%AA%E0%B5%8D%E0%B4%B7%E0%B5%BB</t>
-  </si>
-  <si>
-    <t>https://it.wikipedia.org/wiki/Crittografia_end-to-end</t>
-  </si>
-  <si>
-    <t>https://foundation.wikimedia.org/wiki/Special:MyLanguage/Policy:Privacy_policy/es</t>
-  </si>
-  <si>
-    <t>https://ssd.eff.org/en/module/how-use-otr-windows</t>
-  </si>
-  <si>
-    <t>https://www.schneier.com/blog/archives/2013/10/air_gaps.html</t>
-  </si>
-  <si>
-    <t>https://www.wired.com/2015/10/mr-robot-uses-protonmail-still-isnt-fully-secure/</t>
-  </si>
-  <si>
-    <t>https://foundation.wikimedia.org/wiki/Special:MyLanguage/Policy:Cookie_statement/es</t>
-  </si>
-  <si>
-    <t>https://cpj.org/blog/2016/05/why-telegrams-security-flaws-may-put-irans-journal.php</t>
-  </si>
-  <si>
-    <t>https://nl.wikipedia.org/wiki/End-to-end-encryptie</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/1999/xlink</t>
-  </si>
-  <si>
-    <t>https://ssd.eff.org/en/glossary/end-end-encryption</t>
-  </si>
-  <si>
-    <t>https://pt.wikipedia.org/wiki/Criptografia_de_ponta-a-ponta</t>
-  </si>
-  <si>
-    <t>https://id.wikipedia.org/wiki/Enkripsi_ujung_ke_ujung</t>
-  </si>
-  <si>
-    <t>https://ko.wikipedia.org/wiki/%EB%8B%A8%EB%8C%80%EB%8B%A8_%EC%95%94%ED%98%B8%ED%99%94</t>
-  </si>
-  <si>
-    <t>https://foundation.wikimedia.org/wiki/Policy:Terms_of_Use/es</t>
-  </si>
-  <si>
-    <t>https://creativecommons.org/licenses/by-sa/4.0/deed.es</t>
-  </si>
-  <si>
-    <t>https://upload.wikimedia.org/wikipedia/commons/8/86/Wikipedia_Mes_de_Asia_Banner.svg</t>
-  </si>
-  <si>
-    <t>https://es.wikipedia.org/w/index.php?title=Cifrado_de_extremo_a_extremo&amp;amp;oldid=163332720</t>
-  </si>
-  <si>
-    <t>https://login.wikimedia.org/wiki/Special:CentralAutoLogin/start?type=1x1</t>
-  </si>
-  <si>
-    <t>https://theintercept.com/2015/12/21/democratic-debate-spawns-fantasy-talk-on-encryption/</t>
-  </si>
-  <si>
-    <t>https://he.wikipedia.org/wiki/%D7%94%D7%A6%D7%A4%D7%A0%D7%94_%D7%9E%D7%A7%D7%A6%D7%94-%D7%9C%D7%A7%D7%A6%D7%94</t>
-  </si>
-  <si>
-    <t>https://eu.wikipedia.org/wiki/Ertzetik_ertzerako_zifratze</t>
-  </si>
-  <si>
-    <t>https://foundation.wikimedia.org/wiki/Special:MyLanguage/Policy:Universal_Code_of_Conduct</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2000/svg</t>
-  </si>
-  <si>
-    <t>https://de.wikipedia.org/wiki/Ende-zu-Ende-Verschl%C3%BCsselung</t>
-  </si>
-  <si>
-    <t>https://es.wikipedia.org/wiki/Wikipedia:Mes_de_Asia/2024</t>
-  </si>
-  <si>
-    <t>https://da.wikipedia.org/wiki/End-to-end-kryptering</t>
-  </si>
-  <si>
-    <t>https://pl.wikipedia.org/wiki/Szyfrowanie_od_ko%C5%84ca_do_ko%C5%84ca</t>
-  </si>
-  <si>
-    <t>https://cypherpunks.ca/~iang/pubs/impauth.pdf</t>
-  </si>
-  <si>
-    <t>http://fortune.com/2016/05/21/google-allo-privacy-2/</t>
-  </si>
-  <si>
-    <t>https://www.wikidata.org/wiki/Special:EntityPage/Q1340257#sitelinks-wikipedia</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/End-to-end_encryption</t>
-  </si>
-  <si>
-    <t>https://github.com/maqp/tfc&lt;/a</t>
-  </si>
-  <si>
-    <t>https://www.whonix.org/wiki/Air_Gapped_OpenPGP_Key</t>
-  </si>
-  <si>
-    <t>https://archive.org/details/cryptographyengi00ferg/page/n211</t>
-  </si>
-  <si>
-    <t>https://tr.wikipedia.org/wiki/U%C3%A7tan_uca_%C5%9Fifreleme</t>
-  </si>
-  <si>
-    <t>https://www.theguardian.com/world/2013/jul/11/microsoft-nsa-collaboration-user-data</t>
-  </si>
-  <si>
-    <t>https://dx.doi.org/10.1145%2F1314333.1314340</t>
-  </si>
-  <si>
-    <t>https://cs.wikipedia.org/wiki/Koncov%C3%A9_%C5%A1ifrov%C3%A1n%C3%AD</t>
-  </si>
-  <si>
-    <t>https://web.archive.org/web/20161001160110/https://pep.foundation/docs/pEp-whitepaper.pdf</t>
-  </si>
-  <si>
-    <t>https://es.wikipedia.org/wiki/Cifrado_de_extremo_a_extremo</t>
-  </si>
-  <si>
-    <t>https://developer.wikimedia.org</t>
   </si>
 </sst>
 </file>
@@ -804,128 +804,128 @@
         <v>35</v>
       </c>
     </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="38" spans="1:1">
       <c r="A38" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1021,7 +1021,7 @@
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
     <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6" location="/es.wikipedia.org"/>
+    <hyperlink ref="A7" r:id="rId6"/>
     <hyperlink ref="A8" r:id="rId7"/>
     <hyperlink ref="A9" r:id="rId8"/>
     <hyperlink ref="A10" r:id="rId9"/>
@@ -1046,42 +1046,42 @@
     <hyperlink ref="A29" r:id="rId28"/>
     <hyperlink ref="A30" r:id="rId29"/>
     <hyperlink ref="A31" r:id="rId30"/>
-    <hyperlink ref="A32" r:id="rId31"/>
+    <hyperlink ref="A32" r:id="rId31" location="/es.wikipedia.org"/>
     <hyperlink ref="A33" r:id="rId32"/>
     <hyperlink ref="A34" r:id="rId33"/>
     <hyperlink ref="A35" r:id="rId34"/>
     <hyperlink ref="A36" r:id="rId35"/>
-    <hyperlink ref="A38" r:id="rId36"/>
-    <hyperlink ref="A39" r:id="rId37"/>
-    <hyperlink ref="A40" r:id="rId38"/>
-    <hyperlink ref="A41" r:id="rId39"/>
-    <hyperlink ref="A42" r:id="rId40"/>
-    <hyperlink ref="A43" r:id="rId41"/>
-    <hyperlink ref="A44" r:id="rId42"/>
-    <hyperlink ref="A45" r:id="rId43"/>
-    <hyperlink ref="A46" r:id="rId44"/>
-    <hyperlink ref="A47" r:id="rId45"/>
-    <hyperlink ref="A48" r:id="rId46"/>
-    <hyperlink ref="A49" r:id="rId47"/>
-    <hyperlink ref="A50" r:id="rId48"/>
-    <hyperlink ref="A51" r:id="rId49"/>
-    <hyperlink ref="A52" r:id="rId50"/>
-    <hyperlink ref="A53" r:id="rId51"/>
-    <hyperlink ref="A54" r:id="rId52"/>
-    <hyperlink ref="A55" r:id="rId53"/>
-    <hyperlink ref="A56" r:id="rId54"/>
-    <hyperlink ref="A57" r:id="rId55"/>
-    <hyperlink ref="A58" r:id="rId56"/>
-    <hyperlink ref="A59" r:id="rId57"/>
-    <hyperlink ref="A60" r:id="rId58"/>
-    <hyperlink ref="A61" r:id="rId59"/>
-    <hyperlink ref="A62" r:id="rId60"/>
+    <hyperlink ref="A37" r:id="rId36"/>
+    <hyperlink ref="A38" r:id="rId37"/>
+    <hyperlink ref="A39" r:id="rId38"/>
+    <hyperlink ref="A40" r:id="rId39"/>
+    <hyperlink ref="A41" r:id="rId40"/>
+    <hyperlink ref="A42" r:id="rId41"/>
+    <hyperlink ref="A43" r:id="rId42"/>
+    <hyperlink ref="A44" r:id="rId43" location="sitelinks-wikipedia"/>
+    <hyperlink ref="A45" r:id="rId44"/>
+    <hyperlink ref="A46" r:id="rId45"/>
+    <hyperlink ref="A47" r:id="rId46"/>
+    <hyperlink ref="A48" r:id="rId47"/>
+    <hyperlink ref="A49" r:id="rId48"/>
+    <hyperlink ref="A50" r:id="rId49"/>
+    <hyperlink ref="A51" r:id="rId50"/>
+    <hyperlink ref="A52" r:id="rId51"/>
+    <hyperlink ref="A53" r:id="rId52"/>
+    <hyperlink ref="A54" r:id="rId53"/>
+    <hyperlink ref="A55" r:id="rId54"/>
+    <hyperlink ref="A56" r:id="rId55"/>
+    <hyperlink ref="A57" r:id="rId56"/>
+    <hyperlink ref="A58" r:id="rId57"/>
+    <hyperlink ref="A59" r:id="rId58"/>
+    <hyperlink ref="A60" r:id="rId59"/>
+    <hyperlink ref="A61" r:id="rId60"/>
     <hyperlink ref="A63" r:id="rId61"/>
     <hyperlink ref="A64" r:id="rId62"/>
     <hyperlink ref="A65" r:id="rId63"/>
     <hyperlink ref="A66" r:id="rId64"/>
     <hyperlink ref="A67" r:id="rId65"/>
-    <hyperlink ref="A68" r:id="rId66" location="sitelinks-wikipedia"/>
+    <hyperlink ref="A68" r:id="rId66"/>
     <hyperlink ref="A69" r:id="rId67"/>
     <hyperlink ref="A70" r:id="rId68"/>
     <hyperlink ref="A71" r:id="rId69"/>

</xml_diff>